<commit_message>
feat: actualizar ruta del archivo PDF y agregar nuevos registros de errores en errores.txt
</commit_message>
<xml_diff>
--- a/patchApiSma/articulos.xlsx
+++ b/patchApiSma/articulos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\scripts\patchApiSma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A319402E-024A-4B47-8A8A-7365E6800E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEADBF3B-460A-4BE8-B6FB-731521F2DE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11295" xr2:uid="{FA95EDA8-3678-4D49-8F78-8070BDF73C5E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FA95EDA8-3678-4D49-8F78-8070BDF73C5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,1635 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7655" uniqueCount="7655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7113" uniqueCount="7113">
   <si>
     <t>articulos</t>
-  </si>
-  <si>
-    <t>02040513884</t>
-  </si>
-  <si>
-    <t>02040513933</t>
-  </si>
-  <si>
-    <t>02040515039</t>
-  </si>
-  <si>
-    <t>02040515040</t>
-  </si>
-  <si>
-    <t>02040515041</t>
-  </si>
-  <si>
-    <t>02040515042</t>
-  </si>
-  <si>
-    <t>02040515043</t>
-  </si>
-  <si>
-    <t>02040515044</t>
-  </si>
-  <si>
-    <t>02040515045</t>
-  </si>
-  <si>
-    <t>02040515046</t>
-  </si>
-  <si>
-    <t>02040515048</t>
-  </si>
-  <si>
-    <t>02040515049</t>
-  </si>
-  <si>
-    <t>02040515051</t>
-  </si>
-  <si>
-    <t>02040515052</t>
-  </si>
-  <si>
-    <t>02040515053</t>
-  </si>
-  <si>
-    <t>02040515054</t>
-  </si>
-  <si>
-    <t>02040601518</t>
-  </si>
-  <si>
-    <t>02040601584</t>
-  </si>
-  <si>
-    <t>02040601694</t>
-  </si>
-  <si>
-    <t>02040604569</t>
-  </si>
-  <si>
-    <t>02040604707</t>
-  </si>
-  <si>
-    <t>02040604883</t>
-  </si>
-  <si>
-    <t>02040606231</t>
-  </si>
-  <si>
-    <t>02040606690</t>
-  </si>
-  <si>
-    <t>02040609028</t>
-  </si>
-  <si>
-    <t>02040609032</t>
-  </si>
-  <si>
-    <t>02040609180</t>
-  </si>
-  <si>
-    <t>02040609197</t>
-  </si>
-  <si>
-    <t>02040609396</t>
-  </si>
-  <si>
-    <t>02040609504</t>
-  </si>
-  <si>
-    <t>02040609635</t>
-  </si>
-  <si>
-    <t>02040609641</t>
-  </si>
-  <si>
-    <t>02040609682</t>
-  </si>
-  <si>
-    <t>02040609797</t>
-  </si>
-  <si>
-    <t>02040609898</t>
-  </si>
-  <si>
-    <t>02040609903</t>
-  </si>
-  <si>
-    <t>02040610012</t>
-  </si>
-  <si>
-    <t>02040610299</t>
-  </si>
-  <si>
-    <t>02040610774</t>
-  </si>
-  <si>
-    <t>02040610780</t>
-  </si>
-  <si>
-    <t>02040610807</t>
-  </si>
-  <si>
-    <t>02040610808</t>
-  </si>
-  <si>
-    <t>02040610985</t>
-  </si>
-  <si>
-    <t>02040610987</t>
-  </si>
-  <si>
-    <t>02040610988</t>
-  </si>
-  <si>
-    <t>02040611011</t>
-  </si>
-  <si>
-    <t>02040611012</t>
-  </si>
-  <si>
-    <t>02040611013</t>
-  </si>
-  <si>
-    <t>02040611014</t>
-  </si>
-  <si>
-    <t>02040611062</t>
-  </si>
-  <si>
-    <t>02040611171</t>
-  </si>
-  <si>
-    <t>02040611203</t>
-  </si>
-  <si>
-    <t>02040611247</t>
-  </si>
-  <si>
-    <t>02040611249</t>
-  </si>
-  <si>
-    <t>02040611262</t>
-  </si>
-  <si>
-    <t>02040611264</t>
-  </si>
-  <si>
-    <t>02040611286</t>
-  </si>
-  <si>
-    <t>02040611346</t>
-  </si>
-  <si>
-    <t>02040611364</t>
-  </si>
-  <si>
-    <t>02040611365</t>
-  </si>
-  <si>
-    <t>02040611369</t>
-  </si>
-  <si>
-    <t>02040611448</t>
-  </si>
-  <si>
-    <t>02040611449</t>
-  </si>
-  <si>
-    <t>02040611571</t>
-  </si>
-  <si>
-    <t>02040611573</t>
-  </si>
-  <si>
-    <t>02040611574</t>
-  </si>
-  <si>
-    <t>02040611576</t>
-  </si>
-  <si>
-    <t>02040611583</t>
-  </si>
-  <si>
-    <t>02040611617</t>
-  </si>
-  <si>
-    <t>02040611684</t>
-  </si>
-  <si>
-    <t>02040611685</t>
-  </si>
-  <si>
-    <t>02040611955</t>
-  </si>
-  <si>
-    <t>02040612232</t>
-  </si>
-  <si>
-    <t>02040612277</t>
-  </si>
-  <si>
-    <t>02040612279</t>
-  </si>
-  <si>
-    <t>02040612366</t>
-  </si>
-  <si>
-    <t>02040612519</t>
-  </si>
-  <si>
-    <t>02040612549</t>
-  </si>
-  <si>
-    <t>02040612580</t>
-  </si>
-  <si>
-    <t>02040612585</t>
-  </si>
-  <si>
-    <t>02040612607</t>
-  </si>
-  <si>
-    <t>02040612793</t>
-  </si>
-  <si>
-    <t>02040612807</t>
-  </si>
-  <si>
-    <t>02040612841</t>
-  </si>
-  <si>
-    <t>02040612889</t>
-  </si>
-  <si>
-    <t>02040612933</t>
-  </si>
-  <si>
-    <t>02040613111</t>
-  </si>
-  <si>
-    <t>02040613119</t>
-  </si>
-  <si>
-    <t>02040613278</t>
-  </si>
-  <si>
-    <t>02040613304</t>
-  </si>
-  <si>
-    <t>02040613350</t>
-  </si>
-  <si>
-    <t>02040613594</t>
-  </si>
-  <si>
-    <t>02040614082</t>
-  </si>
-  <si>
-    <t>02040614364</t>
-  </si>
-  <si>
-    <t>02040614365</t>
-  </si>
-  <si>
-    <t>02040614428</t>
-  </si>
-  <si>
-    <t>02040614723</t>
-  </si>
-  <si>
-    <t>02040614912</t>
-  </si>
-  <si>
-    <t>02040615357</t>
-  </si>
-  <si>
-    <t>02040615370</t>
-  </si>
-  <si>
-    <t>02040615541</t>
-  </si>
-  <si>
-    <t>02040615542</t>
-  </si>
-  <si>
-    <t>02040615543</t>
-  </si>
-  <si>
-    <t>02040615544</t>
-  </si>
-  <si>
-    <t>02040615545</t>
-  </si>
-  <si>
-    <t>02040615547</t>
-  </si>
-  <si>
-    <t>02040615548</t>
-  </si>
-  <si>
-    <t>02040615549</t>
-  </si>
-  <si>
-    <t>02040615550</t>
-  </si>
-  <si>
-    <t>02040615551</t>
-  </si>
-  <si>
-    <t>02040615552</t>
-  </si>
-  <si>
-    <t>02040615553</t>
-  </si>
-  <si>
-    <t>02040615554</t>
-  </si>
-  <si>
-    <t>02040615556</t>
-  </si>
-  <si>
-    <t>02040615557</t>
-  </si>
-  <si>
-    <t>02040615558</t>
-  </si>
-  <si>
-    <t>02040615559</t>
-  </si>
-  <si>
-    <t>02040615562</t>
-  </si>
-  <si>
-    <t>02040615564</t>
-  </si>
-  <si>
-    <t>02040615566</t>
-  </si>
-  <si>
-    <t>02040615567</t>
-  </si>
-  <si>
-    <t>02040615568</t>
-  </si>
-  <si>
-    <t>02040615569</t>
-  </si>
-  <si>
-    <t>02040615570</t>
-  </si>
-  <si>
-    <t>02040615571</t>
-  </si>
-  <si>
-    <t>02040615572</t>
-  </si>
-  <si>
-    <t>02040615573</t>
-  </si>
-  <si>
-    <t>02040615574</t>
-  </si>
-  <si>
-    <t>02040615575</t>
-  </si>
-  <si>
-    <t>02040615576</t>
-  </si>
-  <si>
-    <t>02040615577</t>
-  </si>
-  <si>
-    <t>02040615578</t>
-  </si>
-  <si>
-    <t>02040615579</t>
-  </si>
-  <si>
-    <t>02040615580</t>
-  </si>
-  <si>
-    <t>02040615581</t>
-  </si>
-  <si>
-    <t>02040615582</t>
-  </si>
-  <si>
-    <t>02040615583</t>
-  </si>
-  <si>
-    <t>02040615584</t>
-  </si>
-  <si>
-    <t>02040615585</t>
-  </si>
-  <si>
-    <t>02040615586</t>
-  </si>
-  <si>
-    <t>02040615587</t>
-  </si>
-  <si>
-    <t>02040615588</t>
-  </si>
-  <si>
-    <t>02040615589</t>
-  </si>
-  <si>
-    <t>02040615590</t>
-  </si>
-  <si>
-    <t>02040615591</t>
-  </si>
-  <si>
-    <t>02040615592</t>
-  </si>
-  <si>
-    <t>02040615595</t>
-  </si>
-  <si>
-    <t>02040615596</t>
-  </si>
-  <si>
-    <t>02040615597</t>
-  </si>
-  <si>
-    <t>02040615598</t>
-  </si>
-  <si>
-    <t>02040615599</t>
-  </si>
-  <si>
-    <t>02040615601</t>
-  </si>
-  <si>
-    <t>02040615602</t>
-  </si>
-  <si>
-    <t>02040615603</t>
-  </si>
-  <si>
-    <t>02040615604</t>
-  </si>
-  <si>
-    <t>02040615605</t>
-  </si>
-  <si>
-    <t>02040615606</t>
-  </si>
-  <si>
-    <t>02040615607</t>
-  </si>
-  <si>
-    <t>02040615608</t>
-  </si>
-  <si>
-    <t>02040615609</t>
-  </si>
-  <si>
-    <t>02040615610</t>
-  </si>
-  <si>
-    <t>02040615611</t>
-  </si>
-  <si>
-    <t>02040615612</t>
-  </si>
-  <si>
-    <t>02040615613</t>
-  </si>
-  <si>
-    <t>02040615614</t>
-  </si>
-  <si>
-    <t>02040615615</t>
-  </si>
-  <si>
-    <t>02040615616</t>
-  </si>
-  <si>
-    <t>02040615617</t>
-  </si>
-  <si>
-    <t>02040615618</t>
-  </si>
-  <si>
-    <t>02040615619</t>
-  </si>
-  <si>
-    <t>02040615621</t>
-  </si>
-  <si>
-    <t>02040615622</t>
-  </si>
-  <si>
-    <t>02040615623</t>
-  </si>
-  <si>
-    <t>02040615625</t>
-  </si>
-  <si>
-    <t>02040615626</t>
-  </si>
-  <si>
-    <t>02040708517</t>
-  </si>
-  <si>
-    <t>02040709752</t>
-  </si>
-  <si>
-    <t>02040709753</t>
-  </si>
-  <si>
-    <t>02040709763</t>
-  </si>
-  <si>
-    <t>02040709764</t>
-  </si>
-  <si>
-    <t>02040709810</t>
-  </si>
-  <si>
-    <t>02040709811</t>
-  </si>
-  <si>
-    <t>02040711183</t>
-  </si>
-  <si>
-    <t>02040711521</t>
-  </si>
-  <si>
-    <t>02040711522</t>
-  </si>
-  <si>
-    <t>02040711523</t>
-  </si>
-  <si>
-    <t>02040711524</t>
-  </si>
-  <si>
-    <t>02040711525</t>
-  </si>
-  <si>
-    <t>02040711526</t>
-  </si>
-  <si>
-    <t>02040711527</t>
-  </si>
-  <si>
-    <t>02040711528</t>
-  </si>
-  <si>
-    <t>02040711968</t>
-  </si>
-  <si>
-    <t>02040712916</t>
-  </si>
-  <si>
-    <t>02040713003</t>
-  </si>
-  <si>
-    <t>02040713934</t>
-  </si>
-  <si>
-    <t>02040713935</t>
-  </si>
-  <si>
-    <t>02040713964</t>
-  </si>
-  <si>
-    <t>02040713965</t>
-  </si>
-  <si>
-    <t>02040715355</t>
-  </si>
-  <si>
-    <t>02040715371</t>
-  </si>
-  <si>
-    <t>02040715372</t>
-  </si>
-  <si>
-    <t>02040715373</t>
-  </si>
-  <si>
-    <t>02040715374</t>
-  </si>
-  <si>
-    <t>02040715375</t>
-  </si>
-  <si>
-    <t>02040715376</t>
-  </si>
-  <si>
-    <t>02040715377</t>
-  </si>
-  <si>
-    <t>02040715378</t>
-  </si>
-  <si>
-    <t>02040715379</t>
-  </si>
-  <si>
-    <t>02040715380</t>
-  </si>
-  <si>
-    <t>02040715381</t>
-  </si>
-  <si>
-    <t>02040715382</t>
-  </si>
-  <si>
-    <t>02040715383</t>
-  </si>
-  <si>
-    <t>02040806364</t>
-  </si>
-  <si>
-    <t>02040808157</t>
-  </si>
-  <si>
-    <t>02040808915</t>
-  </si>
-  <si>
-    <t>02040809195</t>
-  </si>
-  <si>
-    <t>02040809693</t>
-  </si>
-  <si>
-    <t>02040810226</t>
-  </si>
-  <si>
-    <t>02040810606</t>
-  </si>
-  <si>
-    <t>02040810646</t>
-  </si>
-  <si>
-    <t>02040810647</t>
-  </si>
-  <si>
-    <t>02040810877</t>
-  </si>
-  <si>
-    <t>02040810971</t>
-  </si>
-  <si>
-    <t>02040811280</t>
-  </si>
-  <si>
-    <t>02040811394</t>
-  </si>
-  <si>
-    <t>02040811420</t>
-  </si>
-  <si>
-    <t>02040811546</t>
-  </si>
-  <si>
-    <t>02040811629</t>
-  </si>
-  <si>
-    <t>02040811775</t>
-  </si>
-  <si>
-    <t>02040811799</t>
-  </si>
-  <si>
-    <t>02040811847</t>
-  </si>
-  <si>
-    <t>02040811992</t>
-  </si>
-  <si>
-    <t>02040812421</t>
-  </si>
-  <si>
-    <t>02040812538</t>
-  </si>
-  <si>
-    <t>02040812631</t>
-  </si>
-  <si>
-    <t>02040812881</t>
-  </si>
-  <si>
-    <t>02040813147</t>
-  </si>
-  <si>
-    <t>02040814072</t>
-  </si>
-  <si>
-    <t>02040814073</t>
-  </si>
-  <si>
-    <t>02040814109</t>
-  </si>
-  <si>
-    <t>02040814182</t>
-  </si>
-  <si>
-    <t>02040814294</t>
-  </si>
-  <si>
-    <t>02040814371</t>
-  </si>
-  <si>
-    <t>02040814529</t>
-  </si>
-  <si>
-    <t>02040814560</t>
-  </si>
-  <si>
-    <t>02040814601</t>
-  </si>
-  <si>
-    <t>02040814819</t>
-  </si>
-  <si>
-    <t>02040815020</t>
-  </si>
-  <si>
-    <t>02040815021</t>
-  </si>
-  <si>
-    <t>02040815023</t>
-  </si>
-  <si>
-    <t>02040815024</t>
-  </si>
-  <si>
-    <t>02040815025</t>
-  </si>
-  <si>
-    <t>02040815026</t>
-  </si>
-  <si>
-    <t>02040815027</t>
-  </si>
-  <si>
-    <t>02040815028</t>
-  </si>
-  <si>
-    <t>02040815029</t>
-  </si>
-  <si>
-    <t>02040815030</t>
-  </si>
-  <si>
-    <t>02040815031</t>
-  </si>
-  <si>
-    <t>02040815032</t>
-  </si>
-  <si>
-    <t>02040815033</t>
-  </si>
-  <si>
-    <t>02040815034</t>
-  </si>
-  <si>
-    <t>02040815035</t>
-  </si>
-  <si>
-    <t>02040815036</t>
-  </si>
-  <si>
-    <t>02040815037</t>
-  </si>
-  <si>
-    <t>02040815041</t>
-  </si>
-  <si>
-    <t>02040815042</t>
-  </si>
-  <si>
-    <t>02040815043</t>
-  </si>
-  <si>
-    <t>02040815044</t>
-  </si>
-  <si>
-    <t>02040815047</t>
-  </si>
-  <si>
-    <t>02040815048</t>
-  </si>
-  <si>
-    <t>02040815049</t>
-  </si>
-  <si>
-    <t>02040815050</t>
-  </si>
-  <si>
-    <t>02040815051</t>
-  </si>
-  <si>
-    <t>02040815052</t>
-  </si>
-  <si>
-    <t>02040815053</t>
-  </si>
-  <si>
-    <t>02040815054</t>
-  </si>
-  <si>
-    <t>02040815055</t>
-  </si>
-  <si>
-    <t>02040815056</t>
-  </si>
-  <si>
-    <t>02040815057</t>
-  </si>
-  <si>
-    <t>02040815058</t>
-  </si>
-  <si>
-    <t>02040815059</t>
-  </si>
-  <si>
-    <t>02040815060</t>
-  </si>
-  <si>
-    <t>02040815061</t>
-  </si>
-  <si>
-    <t>02040815063</t>
-  </si>
-  <si>
-    <t>02040815064</t>
-  </si>
-  <si>
-    <t>02040815065</t>
-  </si>
-  <si>
-    <t>02040815067</t>
-  </si>
-  <si>
-    <t>02040815069</t>
-  </si>
-  <si>
-    <t>02040815071</t>
-  </si>
-  <si>
-    <t>02040815072</t>
-  </si>
-  <si>
-    <t>02040815073</t>
-  </si>
-  <si>
-    <t>02040815074</t>
-  </si>
-  <si>
-    <t>02040815075</t>
-  </si>
-  <si>
-    <t>02040815076</t>
-  </si>
-  <si>
-    <t>02040815077</t>
-  </si>
-  <si>
-    <t>02040815078</t>
-  </si>
-  <si>
-    <t>02040815081</t>
-  </si>
-  <si>
-    <t>02040815083</t>
-  </si>
-  <si>
-    <t>02040815084</t>
-  </si>
-  <si>
-    <t>02040815085</t>
-  </si>
-  <si>
-    <t>02040815086</t>
-  </si>
-  <si>
-    <t>02040815087</t>
-  </si>
-  <si>
-    <t>02040815088</t>
-  </si>
-  <si>
-    <t>02040815089</t>
-  </si>
-  <si>
-    <t>02040815091</t>
-  </si>
-  <si>
-    <t>02040900866</t>
-  </si>
-  <si>
-    <t>02040900924</t>
-  </si>
-  <si>
-    <t>02040901133</t>
-  </si>
-  <si>
-    <t>02040901170</t>
-  </si>
-  <si>
-    <t>02040901205</t>
-  </si>
-  <si>
-    <t>02040901210</t>
-  </si>
-  <si>
-    <t>02040901220</t>
-  </si>
-  <si>
-    <t>02040901264</t>
-  </si>
-  <si>
-    <t>02040901857</t>
-  </si>
-  <si>
-    <t>02040902141</t>
-  </si>
-  <si>
-    <t>02040902144</t>
-  </si>
-  <si>
-    <t>02040902805</t>
-  </si>
-  <si>
-    <t>02040903201</t>
-  </si>
-  <si>
-    <t>02040903506</t>
-  </si>
-  <si>
-    <t>02040904643</t>
-  </si>
-  <si>
-    <t>02040904723</t>
-  </si>
-  <si>
-    <t>02040905392</t>
-  </si>
-  <si>
-    <t>02040907817</t>
-  </si>
-  <si>
-    <t>02040909187</t>
-  </si>
-  <si>
-    <t>02040909224</t>
-  </si>
-  <si>
-    <t>02040909226</t>
-  </si>
-  <si>
-    <t>02040909227</t>
-  </si>
-  <si>
-    <t>02040909473</t>
-  </si>
-  <si>
-    <t>02040909501</t>
-  </si>
-  <si>
-    <t>02040909902</t>
-  </si>
-  <si>
-    <t>02040910066</t>
-  </si>
-  <si>
-    <t>02040910225</t>
-  </si>
-  <si>
-    <t>02040910228</t>
-  </si>
-  <si>
-    <t>02040910475</t>
-  </si>
-  <si>
-    <t>02040910528</t>
-  </si>
-  <si>
-    <t>02040910793</t>
-  </si>
-  <si>
-    <t>02040910806</t>
-  </si>
-  <si>
-    <t>02040910833</t>
-  </si>
-  <si>
-    <t>02040910893</t>
-  </si>
-  <si>
-    <t>02040910904</t>
-  </si>
-  <si>
-    <t>02040910978</t>
-  </si>
-  <si>
-    <t>02040911010</t>
-  </si>
-  <si>
-    <t>02040911056</t>
-  </si>
-  <si>
-    <t>02040911080</t>
-  </si>
-  <si>
-    <t>02040911279</t>
-  </si>
-  <si>
-    <t>02040911283</t>
-  </si>
-  <si>
-    <t>02040911368</t>
-  </si>
-  <si>
-    <t>02040911383</t>
-  </si>
-  <si>
-    <t>02040911653</t>
-  </si>
-  <si>
-    <t>02040911673</t>
-  </si>
-  <si>
-    <t>02040911774</t>
-  </si>
-  <si>
-    <t>02040911805</t>
-  </si>
-  <si>
-    <t>02040911846</t>
-  </si>
-  <si>
-    <t>02040911919</t>
-  </si>
-  <si>
-    <t>02040911993</t>
-  </si>
-  <si>
-    <t>02040912038</t>
-  </si>
-  <si>
-    <t>02040912043</t>
-  </si>
-  <si>
-    <t>02040912193</t>
-  </si>
-  <si>
-    <t>02040912194</t>
-  </si>
-  <si>
-    <t>02040912226</t>
-  </si>
-  <si>
-    <t>02040912490</t>
-  </si>
-  <si>
-    <t>02040912579</t>
-  </si>
-  <si>
-    <t>02040912638</t>
-  </si>
-  <si>
-    <t>02040912639</t>
-  </si>
-  <si>
-    <t>02040912792</t>
-  </si>
-  <si>
-    <t>02040912880</t>
-  </si>
-  <si>
-    <t>02040912888</t>
-  </si>
-  <si>
-    <t>02040912896</t>
-  </si>
-  <si>
-    <t>02040913047</t>
-  </si>
-  <si>
-    <t>02040913129</t>
-  </si>
-  <si>
-    <t>02040913130</t>
-  </si>
-  <si>
-    <t>02040913132</t>
-  </si>
-  <si>
-    <t>02040913146</t>
-  </si>
-  <si>
-    <t>02040913249</t>
-  </si>
-  <si>
-    <t>02040913310</t>
-  </si>
-  <si>
-    <t>02040913448</t>
-  </si>
-  <si>
-    <t>02040913561</t>
-  </si>
-  <si>
-    <t>02040913708</t>
-  </si>
-  <si>
-    <t>02040913710</t>
-  </si>
-  <si>
-    <t>02040913735</t>
-  </si>
-  <si>
-    <t>02040914081</t>
-  </si>
-  <si>
-    <t>02040914370</t>
-  </si>
-  <si>
-    <t>02040914449</t>
-  </si>
-  <si>
-    <t>02040914600</t>
-  </si>
-  <si>
-    <t>02040914818</t>
-  </si>
-  <si>
-    <t>02040915015</t>
-  </si>
-  <si>
-    <t>02040915018</t>
-  </si>
-  <si>
-    <t>02040915346</t>
-  </si>
-  <si>
-    <t>02040915356</t>
-  </si>
-  <si>
-    <t>02040915367</t>
-  </si>
-  <si>
-    <t>02040915368</t>
-  </si>
-  <si>
-    <t>02040915369</t>
-  </si>
-  <si>
-    <t>02040915474</t>
-  </si>
-  <si>
-    <t>02040915475</t>
-  </si>
-  <si>
-    <t>02040915476</t>
-  </si>
-  <si>
-    <t>02040915477</t>
-  </si>
-  <si>
-    <t>02040915479</t>
-  </si>
-  <si>
-    <t>02040915481</t>
-  </si>
-  <si>
-    <t>02040915482</t>
-  </si>
-  <si>
-    <t>02040915483</t>
-  </si>
-  <si>
-    <t>02040915484</t>
-  </si>
-  <si>
-    <t>02040915485</t>
-  </si>
-  <si>
-    <t>02040915486</t>
-  </si>
-  <si>
-    <t>02040915487</t>
-  </si>
-  <si>
-    <t>02040915488</t>
-  </si>
-  <si>
-    <t>02040915489</t>
-  </si>
-  <si>
-    <t>02040915490</t>
-  </si>
-  <si>
-    <t>02040915491</t>
-  </si>
-  <si>
-    <t>02040915492</t>
-  </si>
-  <si>
-    <t>02040915493</t>
-  </si>
-  <si>
-    <t>02040915495</t>
-  </si>
-  <si>
-    <t>02040915497</t>
-  </si>
-  <si>
-    <t>02040915498</t>
-  </si>
-  <si>
-    <t>02040915505</t>
-  </si>
-  <si>
-    <t>02040915506</t>
-  </si>
-  <si>
-    <t>02040915508</t>
-  </si>
-  <si>
-    <t>02040915509</t>
-  </si>
-  <si>
-    <t>02040915512</t>
-  </si>
-  <si>
-    <t>02040915513</t>
-  </si>
-  <si>
-    <t>02040915514</t>
-  </si>
-  <si>
-    <t>02040915515</t>
-  </si>
-  <si>
-    <t>02040915516</t>
-  </si>
-  <si>
-    <t>02040915517</t>
-  </si>
-  <si>
-    <t>02040915518</t>
-  </si>
-  <si>
-    <t>02040915519</t>
-  </si>
-  <si>
-    <t>02040915521</t>
-  </si>
-  <si>
-    <t>02040915522</t>
-  </si>
-  <si>
-    <t>02040915523</t>
-  </si>
-  <si>
-    <t>02040915524</t>
-  </si>
-  <si>
-    <t>02040915525</t>
-  </si>
-  <si>
-    <t>02040915526</t>
-  </si>
-  <si>
-    <t>02040915527</t>
-  </si>
-  <si>
-    <t>02040915531</t>
-  </si>
-  <si>
-    <t>02040915532</t>
-  </si>
-  <si>
-    <t>02040915533</t>
-  </si>
-  <si>
-    <t>02040915534</t>
-  </si>
-  <si>
-    <t>02040915535</t>
-  </si>
-  <si>
-    <t>02040915538</t>
-  </si>
-  <si>
-    <t>02040915539</t>
-  </si>
-  <si>
-    <t>02040915540</t>
-  </si>
-  <si>
-    <t>02040915541</t>
-  </si>
-  <si>
-    <t>02040915542</t>
-  </si>
-  <si>
-    <t>02040915543</t>
-  </si>
-  <si>
-    <t>02040915544</t>
-  </si>
-  <si>
-    <t>02040915545</t>
-  </si>
-  <si>
-    <t>02040915546</t>
-  </si>
-  <si>
-    <t>02040915547</t>
-  </si>
-  <si>
-    <t>02040915549</t>
-  </si>
-  <si>
-    <t>02040915550</t>
-  </si>
-  <si>
-    <t>02040915551</t>
-  </si>
-  <si>
-    <t>02040915552</t>
-  </si>
-  <si>
-    <t>02040915554</t>
-  </si>
-  <si>
-    <t>02040915555</t>
-  </si>
-  <si>
-    <t>02040915556</t>
-  </si>
-  <si>
-    <t>02040915557</t>
-  </si>
-  <si>
-    <t>02040915558</t>
-  </si>
-  <si>
-    <t>02040915559</t>
-  </si>
-  <si>
-    <t>02040915560</t>
-  </si>
-  <si>
-    <t>02040915561</t>
-  </si>
-  <si>
-    <t>02040915562</t>
-  </si>
-  <si>
-    <t>02040915563</t>
-  </si>
-  <si>
-    <t>02040915564</t>
-  </si>
-  <si>
-    <t>02040915565</t>
-  </si>
-  <si>
-    <t>02040915566</t>
-  </si>
-  <si>
-    <t>02040915567</t>
-  </si>
-  <si>
-    <t>02040915568</t>
-  </si>
-  <si>
-    <t>02040915569</t>
-  </si>
-  <si>
-    <t>02040915570</t>
-  </si>
-  <si>
-    <t>02040915571</t>
-  </si>
-  <si>
-    <t>02040915572</t>
-  </si>
-  <si>
-    <t>02040915573</t>
-  </si>
-  <si>
-    <t>02040915574</t>
-  </si>
-  <si>
-    <t>02040915575</t>
-  </si>
-  <si>
-    <t>02040915576</t>
-  </si>
-  <si>
-    <t>02040915577</t>
-  </si>
-  <si>
-    <t>02040915578</t>
-  </si>
-  <si>
-    <t>02040915579</t>
-  </si>
-  <si>
-    <t>02040915580</t>
-  </si>
-  <si>
-    <t>02040915581</t>
-  </si>
-  <si>
-    <t>02040915582</t>
-  </si>
-  <si>
-    <t>02040915583</t>
-  </si>
-  <si>
-    <t>02040915584</t>
-  </si>
-  <si>
-    <t>02040915585</t>
-  </si>
-  <si>
-    <t>02040915592</t>
-  </si>
-  <si>
-    <t>02040915593</t>
-  </si>
-  <si>
-    <t>02040915594</t>
-  </si>
-  <si>
-    <t>02040915595</t>
-  </si>
-  <si>
-    <t>02040915596</t>
-  </si>
-  <si>
-    <t>02040915597</t>
-  </si>
-  <si>
-    <t>02040915598</t>
-  </si>
-  <si>
-    <t>02040915599</t>
-  </si>
-  <si>
-    <t>02040915600</t>
-  </si>
-  <si>
-    <t>02040915601</t>
-  </si>
-  <si>
-    <t>02040915602</t>
-  </si>
-  <si>
-    <t>02040915603</t>
-  </si>
-  <si>
-    <t>02040915604</t>
-  </si>
-  <si>
-    <t>02040915605</t>
-  </si>
-  <si>
-    <t>02040915606</t>
-  </si>
-  <si>
-    <t>02040915607</t>
-  </si>
-  <si>
-    <t>02040915608</t>
-  </si>
-  <si>
-    <t>02040915609</t>
-  </si>
-  <si>
-    <t>02040915610</t>
-  </si>
-  <si>
-    <t>02041009558</t>
-  </si>
-  <si>
-    <t>02041110229</t>
-  </si>
-  <si>
-    <t>02041110230</t>
-  </si>
-  <si>
-    <t>02041110231</t>
-  </si>
-  <si>
-    <t>02041204770</t>
-  </si>
-  <si>
-    <t>02041210230</t>
-  </si>
-  <si>
-    <t>02041210559</t>
-  </si>
-  <si>
-    <t>02041210823</t>
-  </si>
-  <si>
-    <t>02041211876</t>
-  </si>
-  <si>
-    <t>02041212048</t>
-  </si>
-  <si>
-    <t>02041212491</t>
-  </si>
-  <si>
-    <t>02041212891</t>
-  </si>
-  <si>
-    <t>02041212897</t>
-  </si>
-  <si>
-    <t>02041213736</t>
-  </si>
-  <si>
-    <t>02041213775</t>
-  </si>
-  <si>
-    <t>02041214108</t>
-  </si>
-  <si>
-    <t>02041214109</t>
-  </si>
-  <si>
-    <t>02041214110</t>
-  </si>
-  <si>
-    <t>02041214111</t>
-  </si>
-  <si>
-    <t>02041214112</t>
-  </si>
-  <si>
-    <t>02041214113</t>
-  </si>
-  <si>
-    <t>02041310773</t>
-  </si>
-  <si>
-    <t>02041411438</t>
-  </si>
-  <si>
-    <t>02041411442</t>
-  </si>
-  <si>
-    <t>02041411596</t>
-  </si>
-  <si>
-    <t>02041411597</t>
-  </si>
-  <si>
-    <t>02041412033</t>
-  </si>
-  <si>
-    <t>02041412696</t>
-  </si>
-  <si>
-    <t>02041412697</t>
-  </si>
-  <si>
-    <t>02041412932</t>
-  </si>
-  <si>
-    <t>02041413243</t>
-  </si>
-  <si>
-    <t>02041413961</t>
-  </si>
-  <si>
-    <t>02041414410</t>
-  </si>
-  <si>
-    <t>02041414527</t>
-  </si>
-  <si>
-    <t>02041414924</t>
-  </si>
-  <si>
-    <t>02041414927</t>
-  </si>
-  <si>
-    <t>02041414930</t>
-  </si>
-  <si>
-    <t>02041414931</t>
-  </si>
-  <si>
-    <t>02041414932</t>
-  </si>
-  <si>
-    <t>02041414934</t>
   </si>
   <si>
     <t>02041414935</t>
@@ -23350,9 +21724,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89429DE1-A58F-47E6-BD2E-5E1F03E2AA87}">
-  <dimension ref="A1:A7655"/>
+  <dimension ref="A1:A7113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7077" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7113"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -58924,2716 +57300,6 @@
         <v>7112</v>
       </c>
     </row>
-    <row r="7114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7114" t="s">
-        <v>7113</v>
-      </c>
-    </row>
-    <row r="7115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7115" t="s">
-        <v>7114</v>
-      </c>
-    </row>
-    <row r="7116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7116" t="s">
-        <v>7115</v>
-      </c>
-    </row>
-    <row r="7117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7117" t="s">
-        <v>7116</v>
-      </c>
-    </row>
-    <row r="7118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7118" t="s">
-        <v>7117</v>
-      </c>
-    </row>
-    <row r="7119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7119" t="s">
-        <v>7118</v>
-      </c>
-    </row>
-    <row r="7120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7120" t="s">
-        <v>7119</v>
-      </c>
-    </row>
-    <row r="7121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7121" t="s">
-        <v>7120</v>
-      </c>
-    </row>
-    <row r="7122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7122" t="s">
-        <v>7121</v>
-      </c>
-    </row>
-    <row r="7123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7123" t="s">
-        <v>7122</v>
-      </c>
-    </row>
-    <row r="7124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7124" t="s">
-        <v>7123</v>
-      </c>
-    </row>
-    <row r="7125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7125" t="s">
-        <v>7124</v>
-      </c>
-    </row>
-    <row r="7126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7126" t="s">
-        <v>7125</v>
-      </c>
-    </row>
-    <row r="7127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7127" t="s">
-        <v>7126</v>
-      </c>
-    </row>
-    <row r="7128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7128" t="s">
-        <v>7127</v>
-      </c>
-    </row>
-    <row r="7129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7129" t="s">
-        <v>7128</v>
-      </c>
-    </row>
-    <row r="7130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7130" t="s">
-        <v>7129</v>
-      </c>
-    </row>
-    <row r="7131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7131" t="s">
-        <v>7130</v>
-      </c>
-    </row>
-    <row r="7132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7132" t="s">
-        <v>7131</v>
-      </c>
-    </row>
-    <row r="7133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7133" t="s">
-        <v>7132</v>
-      </c>
-    </row>
-    <row r="7134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7134" t="s">
-        <v>7133</v>
-      </c>
-    </row>
-    <row r="7135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7135" t="s">
-        <v>7134</v>
-      </c>
-    </row>
-    <row r="7136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7136" t="s">
-        <v>7135</v>
-      </c>
-    </row>
-    <row r="7137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7137" t="s">
-        <v>7136</v>
-      </c>
-    </row>
-    <row r="7138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7138" t="s">
-        <v>7137</v>
-      </c>
-    </row>
-    <row r="7139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7139" t="s">
-        <v>7138</v>
-      </c>
-    </row>
-    <row r="7140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7140" t="s">
-        <v>7139</v>
-      </c>
-    </row>
-    <row r="7141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7141" t="s">
-        <v>7140</v>
-      </c>
-    </row>
-    <row r="7142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7142" t="s">
-        <v>7141</v>
-      </c>
-    </row>
-    <row r="7143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7143" t="s">
-        <v>7142</v>
-      </c>
-    </row>
-    <row r="7144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7144" t="s">
-        <v>7143</v>
-      </c>
-    </row>
-    <row r="7145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7145" t="s">
-        <v>7144</v>
-      </c>
-    </row>
-    <row r="7146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7146" t="s">
-        <v>7145</v>
-      </c>
-    </row>
-    <row r="7147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7147" t="s">
-        <v>7146</v>
-      </c>
-    </row>
-    <row r="7148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7148" t="s">
-        <v>7147</v>
-      </c>
-    </row>
-    <row r="7149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7149" t="s">
-        <v>7148</v>
-      </c>
-    </row>
-    <row r="7150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7150" t="s">
-        <v>7149</v>
-      </c>
-    </row>
-    <row r="7151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7151" t="s">
-        <v>7150</v>
-      </c>
-    </row>
-    <row r="7152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7152" t="s">
-        <v>7151</v>
-      </c>
-    </row>
-    <row r="7153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7153" t="s">
-        <v>7152</v>
-      </c>
-    </row>
-    <row r="7154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7154" t="s">
-        <v>7153</v>
-      </c>
-    </row>
-    <row r="7155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7155" t="s">
-        <v>7154</v>
-      </c>
-    </row>
-    <row r="7156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7156" t="s">
-        <v>7155</v>
-      </c>
-    </row>
-    <row r="7157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7157" t="s">
-        <v>7156</v>
-      </c>
-    </row>
-    <row r="7158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7158" t="s">
-        <v>7157</v>
-      </c>
-    </row>
-    <row r="7159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7159" t="s">
-        <v>7158</v>
-      </c>
-    </row>
-    <row r="7160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7160" t="s">
-        <v>7159</v>
-      </c>
-    </row>
-    <row r="7161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7161" t="s">
-        <v>7160</v>
-      </c>
-    </row>
-    <row r="7162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7162" t="s">
-        <v>7161</v>
-      </c>
-    </row>
-    <row r="7163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7163" t="s">
-        <v>7162</v>
-      </c>
-    </row>
-    <row r="7164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7164" t="s">
-        <v>7163</v>
-      </c>
-    </row>
-    <row r="7165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7165" t="s">
-        <v>7164</v>
-      </c>
-    </row>
-    <row r="7166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7166" t="s">
-        <v>7165</v>
-      </c>
-    </row>
-    <row r="7167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7167" t="s">
-        <v>7166</v>
-      </c>
-    </row>
-    <row r="7168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7168" t="s">
-        <v>7167</v>
-      </c>
-    </row>
-    <row r="7169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7169" t="s">
-        <v>7168</v>
-      </c>
-    </row>
-    <row r="7170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7170" t="s">
-        <v>7169</v>
-      </c>
-    </row>
-    <row r="7171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7171" t="s">
-        <v>7170</v>
-      </c>
-    </row>
-    <row r="7172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7172" t="s">
-        <v>7171</v>
-      </c>
-    </row>
-    <row r="7173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7173" t="s">
-        <v>7172</v>
-      </c>
-    </row>
-    <row r="7174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7174" t="s">
-        <v>7173</v>
-      </c>
-    </row>
-    <row r="7175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7175" t="s">
-        <v>7174</v>
-      </c>
-    </row>
-    <row r="7176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7176" t="s">
-        <v>7175</v>
-      </c>
-    </row>
-    <row r="7177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7177" t="s">
-        <v>7176</v>
-      </c>
-    </row>
-    <row r="7178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7178" t="s">
-        <v>7177</v>
-      </c>
-    </row>
-    <row r="7179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7179" t="s">
-        <v>7178</v>
-      </c>
-    </row>
-    <row r="7180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7180" t="s">
-        <v>7179</v>
-      </c>
-    </row>
-    <row r="7181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7181" t="s">
-        <v>7180</v>
-      </c>
-    </row>
-    <row r="7182" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7182" t="s">
-        <v>7181</v>
-      </c>
-    </row>
-    <row r="7183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7183" t="s">
-        <v>7182</v>
-      </c>
-    </row>
-    <row r="7184" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7184" t="s">
-        <v>7183</v>
-      </c>
-    </row>
-    <row r="7185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7185" t="s">
-        <v>7184</v>
-      </c>
-    </row>
-    <row r="7186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7186" t="s">
-        <v>7185</v>
-      </c>
-    </row>
-    <row r="7187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7187" t="s">
-        <v>7186</v>
-      </c>
-    </row>
-    <row r="7188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7188" t="s">
-        <v>7187</v>
-      </c>
-    </row>
-    <row r="7189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7189" t="s">
-        <v>7188</v>
-      </c>
-    </row>
-    <row r="7190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7190" t="s">
-        <v>7189</v>
-      </c>
-    </row>
-    <row r="7191" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7191" t="s">
-        <v>7190</v>
-      </c>
-    </row>
-    <row r="7192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7192" t="s">
-        <v>7191</v>
-      </c>
-    </row>
-    <row r="7193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7193" t="s">
-        <v>7192</v>
-      </c>
-    </row>
-    <row r="7194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7194" t="s">
-        <v>7193</v>
-      </c>
-    </row>
-    <row r="7195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7195" t="s">
-        <v>7194</v>
-      </c>
-    </row>
-    <row r="7196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7196" t="s">
-        <v>7195</v>
-      </c>
-    </row>
-    <row r="7197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7197" t="s">
-        <v>7196</v>
-      </c>
-    </row>
-    <row r="7198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7198" t="s">
-        <v>7197</v>
-      </c>
-    </row>
-    <row r="7199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7199" t="s">
-        <v>7198</v>
-      </c>
-    </row>
-    <row r="7200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7200" t="s">
-        <v>7199</v>
-      </c>
-    </row>
-    <row r="7201" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7201" t="s">
-        <v>7200</v>
-      </c>
-    </row>
-    <row r="7202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7202" t="s">
-        <v>7201</v>
-      </c>
-    </row>
-    <row r="7203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7203" t="s">
-        <v>7202</v>
-      </c>
-    </row>
-    <row r="7204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7204" t="s">
-        <v>7203</v>
-      </c>
-    </row>
-    <row r="7205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7205" t="s">
-        <v>7204</v>
-      </c>
-    </row>
-    <row r="7206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7206" t="s">
-        <v>7205</v>
-      </c>
-    </row>
-    <row r="7207" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7207" t="s">
-        <v>7206</v>
-      </c>
-    </row>
-    <row r="7208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7208" t="s">
-        <v>7207</v>
-      </c>
-    </row>
-    <row r="7209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7209" t="s">
-        <v>7208</v>
-      </c>
-    </row>
-    <row r="7210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7210" t="s">
-        <v>7209</v>
-      </c>
-    </row>
-    <row r="7211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7211" t="s">
-        <v>7210</v>
-      </c>
-    </row>
-    <row r="7212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7212" t="s">
-        <v>7211</v>
-      </c>
-    </row>
-    <row r="7213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7213" t="s">
-        <v>7212</v>
-      </c>
-    </row>
-    <row r="7214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7214" t="s">
-        <v>7213</v>
-      </c>
-    </row>
-    <row r="7215" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7215" t="s">
-        <v>7214</v>
-      </c>
-    </row>
-    <row r="7216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7216" t="s">
-        <v>7215</v>
-      </c>
-    </row>
-    <row r="7217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7217" t="s">
-        <v>7216</v>
-      </c>
-    </row>
-    <row r="7218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7218" t="s">
-        <v>7217</v>
-      </c>
-    </row>
-    <row r="7219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7219" t="s">
-        <v>7218</v>
-      </c>
-    </row>
-    <row r="7220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7220" t="s">
-        <v>7219</v>
-      </c>
-    </row>
-    <row r="7221" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7221" t="s">
-        <v>7220</v>
-      </c>
-    </row>
-    <row r="7222" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7222" t="s">
-        <v>7221</v>
-      </c>
-    </row>
-    <row r="7223" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7223" t="s">
-        <v>7222</v>
-      </c>
-    </row>
-    <row r="7224" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7224" t="s">
-        <v>7223</v>
-      </c>
-    </row>
-    <row r="7225" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7225" t="s">
-        <v>7224</v>
-      </c>
-    </row>
-    <row r="7226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7226" t="s">
-        <v>7225</v>
-      </c>
-    </row>
-    <row r="7227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7227" t="s">
-        <v>7226</v>
-      </c>
-    </row>
-    <row r="7228" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7228" t="s">
-        <v>7227</v>
-      </c>
-    </row>
-    <row r="7229" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7229" t="s">
-        <v>7228</v>
-      </c>
-    </row>
-    <row r="7230" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7230" t="s">
-        <v>7229</v>
-      </c>
-    </row>
-    <row r="7231" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7231" t="s">
-        <v>7230</v>
-      </c>
-    </row>
-    <row r="7232" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7232" t="s">
-        <v>7231</v>
-      </c>
-    </row>
-    <row r="7233" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7233" t="s">
-        <v>7232</v>
-      </c>
-    </row>
-    <row r="7234" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7234" t="s">
-        <v>7233</v>
-      </c>
-    </row>
-    <row r="7235" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7235" t="s">
-        <v>7234</v>
-      </c>
-    </row>
-    <row r="7236" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7236" t="s">
-        <v>7235</v>
-      </c>
-    </row>
-    <row r="7237" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7237" t="s">
-        <v>7236</v>
-      </c>
-    </row>
-    <row r="7238" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7238" t="s">
-        <v>7237</v>
-      </c>
-    </row>
-    <row r="7239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7239" t="s">
-        <v>7238</v>
-      </c>
-    </row>
-    <row r="7240" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7240" t="s">
-        <v>7239</v>
-      </c>
-    </row>
-    <row r="7241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7241" t="s">
-        <v>7240</v>
-      </c>
-    </row>
-    <row r="7242" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7242" t="s">
-        <v>7241</v>
-      </c>
-    </row>
-    <row r="7243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7243" t="s">
-        <v>7242</v>
-      </c>
-    </row>
-    <row r="7244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7244" t="s">
-        <v>7243</v>
-      </c>
-    </row>
-    <row r="7245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7245" t="s">
-        <v>7244</v>
-      </c>
-    </row>
-    <row r="7246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7246" t="s">
-        <v>7245</v>
-      </c>
-    </row>
-    <row r="7247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7247" t="s">
-        <v>7246</v>
-      </c>
-    </row>
-    <row r="7248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7248" t="s">
-        <v>7247</v>
-      </c>
-    </row>
-    <row r="7249" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7249" t="s">
-        <v>7248</v>
-      </c>
-    </row>
-    <row r="7250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7250" t="s">
-        <v>7249</v>
-      </c>
-    </row>
-    <row r="7251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7251" t="s">
-        <v>7250</v>
-      </c>
-    </row>
-    <row r="7252" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7252" t="s">
-        <v>7251</v>
-      </c>
-    </row>
-    <row r="7253" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7253" t="s">
-        <v>7252</v>
-      </c>
-    </row>
-    <row r="7254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7254" t="s">
-        <v>7253</v>
-      </c>
-    </row>
-    <row r="7255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7255" t="s">
-        <v>7254</v>
-      </c>
-    </row>
-    <row r="7256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7256" t="s">
-        <v>7255</v>
-      </c>
-    </row>
-    <row r="7257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7257" t="s">
-        <v>7256</v>
-      </c>
-    </row>
-    <row r="7258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7258" t="s">
-        <v>7257</v>
-      </c>
-    </row>
-    <row r="7259" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7259" t="s">
-        <v>7258</v>
-      </c>
-    </row>
-    <row r="7260" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7260" t="s">
-        <v>7259</v>
-      </c>
-    </row>
-    <row r="7261" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7261" t="s">
-        <v>7260</v>
-      </c>
-    </row>
-    <row r="7262" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7262" t="s">
-        <v>7261</v>
-      </c>
-    </row>
-    <row r="7263" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7263" t="s">
-        <v>7262</v>
-      </c>
-    </row>
-    <row r="7264" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7264" t="s">
-        <v>7263</v>
-      </c>
-    </row>
-    <row r="7265" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7265" t="s">
-        <v>7264</v>
-      </c>
-    </row>
-    <row r="7266" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7266" t="s">
-        <v>7265</v>
-      </c>
-    </row>
-    <row r="7267" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7267" t="s">
-        <v>7266</v>
-      </c>
-    </row>
-    <row r="7268" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7268" t="s">
-        <v>7267</v>
-      </c>
-    </row>
-    <row r="7269" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7269" t="s">
-        <v>7268</v>
-      </c>
-    </row>
-    <row r="7270" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7270" t="s">
-        <v>7269</v>
-      </c>
-    </row>
-    <row r="7271" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7271" t="s">
-        <v>7270</v>
-      </c>
-    </row>
-    <row r="7272" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7272" t="s">
-        <v>7271</v>
-      </c>
-    </row>
-    <row r="7273" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7273" t="s">
-        <v>7272</v>
-      </c>
-    </row>
-    <row r="7274" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7274" t="s">
-        <v>7273</v>
-      </c>
-    </row>
-    <row r="7275" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7275" t="s">
-        <v>7274</v>
-      </c>
-    </row>
-    <row r="7276" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7276" t="s">
-        <v>7275</v>
-      </c>
-    </row>
-    <row r="7277" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7277" t="s">
-        <v>7276</v>
-      </c>
-    </row>
-    <row r="7278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7278" t="s">
-        <v>7277</v>
-      </c>
-    </row>
-    <row r="7279" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7279" t="s">
-        <v>7278</v>
-      </c>
-    </row>
-    <row r="7280" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7280" t="s">
-        <v>7279</v>
-      </c>
-    </row>
-    <row r="7281" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7281" t="s">
-        <v>7280</v>
-      </c>
-    </row>
-    <row r="7282" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7282" t="s">
-        <v>7281</v>
-      </c>
-    </row>
-    <row r="7283" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7283" t="s">
-        <v>7282</v>
-      </c>
-    </row>
-    <row r="7284" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7284" t="s">
-        <v>7283</v>
-      </c>
-    </row>
-    <row r="7285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7285" t="s">
-        <v>7284</v>
-      </c>
-    </row>
-    <row r="7286" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7286" t="s">
-        <v>7285</v>
-      </c>
-    </row>
-    <row r="7287" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7287" t="s">
-        <v>7286</v>
-      </c>
-    </row>
-    <row r="7288" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7288" t="s">
-        <v>7287</v>
-      </c>
-    </row>
-    <row r="7289" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7289" t="s">
-        <v>7288</v>
-      </c>
-    </row>
-    <row r="7290" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7290" t="s">
-        <v>7289</v>
-      </c>
-    </row>
-    <row r="7291" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7291" t="s">
-        <v>7290</v>
-      </c>
-    </row>
-    <row r="7292" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7292" t="s">
-        <v>7291</v>
-      </c>
-    </row>
-    <row r="7293" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7293" t="s">
-        <v>7292</v>
-      </c>
-    </row>
-    <row r="7294" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7294" t="s">
-        <v>7293</v>
-      </c>
-    </row>
-    <row r="7295" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7295" t="s">
-        <v>7294</v>
-      </c>
-    </row>
-    <row r="7296" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7296" t="s">
-        <v>7295</v>
-      </c>
-    </row>
-    <row r="7297" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7297" t="s">
-        <v>7296</v>
-      </c>
-    </row>
-    <row r="7298" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7298" t="s">
-        <v>7297</v>
-      </c>
-    </row>
-    <row r="7299" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7299" t="s">
-        <v>7298</v>
-      </c>
-    </row>
-    <row r="7300" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7300" t="s">
-        <v>7299</v>
-      </c>
-    </row>
-    <row r="7301" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7301" t="s">
-        <v>7300</v>
-      </c>
-    </row>
-    <row r="7302" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7302" t="s">
-        <v>7301</v>
-      </c>
-    </row>
-    <row r="7303" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7303" t="s">
-        <v>7302</v>
-      </c>
-    </row>
-    <row r="7304" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7304" t="s">
-        <v>7303</v>
-      </c>
-    </row>
-    <row r="7305" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7305" t="s">
-        <v>7304</v>
-      </c>
-    </row>
-    <row r="7306" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7306" t="s">
-        <v>7305</v>
-      </c>
-    </row>
-    <row r="7307" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7307" t="s">
-        <v>7306</v>
-      </c>
-    </row>
-    <row r="7308" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7308" t="s">
-        <v>7307</v>
-      </c>
-    </row>
-    <row r="7309" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7309" t="s">
-        <v>7308</v>
-      </c>
-    </row>
-    <row r="7310" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7310" t="s">
-        <v>7309</v>
-      </c>
-    </row>
-    <row r="7311" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7311" t="s">
-        <v>7310</v>
-      </c>
-    </row>
-    <row r="7312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7312" t="s">
-        <v>7311</v>
-      </c>
-    </row>
-    <row r="7313" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7313" t="s">
-        <v>7312</v>
-      </c>
-    </row>
-    <row r="7314" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7314" t="s">
-        <v>7313</v>
-      </c>
-    </row>
-    <row r="7315" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7315" t="s">
-        <v>7314</v>
-      </c>
-    </row>
-    <row r="7316" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7316" t="s">
-        <v>7315</v>
-      </c>
-    </row>
-    <row r="7317" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7317" t="s">
-        <v>7316</v>
-      </c>
-    </row>
-    <row r="7318" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7318" t="s">
-        <v>7317</v>
-      </c>
-    </row>
-    <row r="7319" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7319" t="s">
-        <v>7318</v>
-      </c>
-    </row>
-    <row r="7320" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7320" t="s">
-        <v>7319</v>
-      </c>
-    </row>
-    <row r="7321" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7321" t="s">
-        <v>7320</v>
-      </c>
-    </row>
-    <row r="7322" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7322" t="s">
-        <v>7321</v>
-      </c>
-    </row>
-    <row r="7323" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7323" t="s">
-        <v>7322</v>
-      </c>
-    </row>
-    <row r="7324" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7324" t="s">
-        <v>7323</v>
-      </c>
-    </row>
-    <row r="7325" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7325" t="s">
-        <v>7324</v>
-      </c>
-    </row>
-    <row r="7326" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7326" t="s">
-        <v>7325</v>
-      </c>
-    </row>
-    <row r="7327" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7327" t="s">
-        <v>7326</v>
-      </c>
-    </row>
-    <row r="7328" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7328" t="s">
-        <v>7327</v>
-      </c>
-    </row>
-    <row r="7329" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7329" t="s">
-        <v>7328</v>
-      </c>
-    </row>
-    <row r="7330" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7330" t="s">
-        <v>7329</v>
-      </c>
-    </row>
-    <row r="7331" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7331" t="s">
-        <v>7330</v>
-      </c>
-    </row>
-    <row r="7332" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7332" t="s">
-        <v>7331</v>
-      </c>
-    </row>
-    <row r="7333" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7333" t="s">
-        <v>7332</v>
-      </c>
-    </row>
-    <row r="7334" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7334" t="s">
-        <v>7333</v>
-      </c>
-    </row>
-    <row r="7335" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7335" t="s">
-        <v>7334</v>
-      </c>
-    </row>
-    <row r="7336" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7336" t="s">
-        <v>7335</v>
-      </c>
-    </row>
-    <row r="7337" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7337" t="s">
-        <v>7336</v>
-      </c>
-    </row>
-    <row r="7338" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7338" t="s">
-        <v>7337</v>
-      </c>
-    </row>
-    <row r="7339" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7339" t="s">
-        <v>7338</v>
-      </c>
-    </row>
-    <row r="7340" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7340" t="s">
-        <v>7339</v>
-      </c>
-    </row>
-    <row r="7341" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7341" t="s">
-        <v>7340</v>
-      </c>
-    </row>
-    <row r="7342" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7342" t="s">
-        <v>7341</v>
-      </c>
-    </row>
-    <row r="7343" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7343" t="s">
-        <v>7342</v>
-      </c>
-    </row>
-    <row r="7344" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7344" t="s">
-        <v>7343</v>
-      </c>
-    </row>
-    <row r="7345" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7345" t="s">
-        <v>7344</v>
-      </c>
-    </row>
-    <row r="7346" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7346" t="s">
-        <v>7345</v>
-      </c>
-    </row>
-    <row r="7347" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7347" t="s">
-        <v>7346</v>
-      </c>
-    </row>
-    <row r="7348" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7348" t="s">
-        <v>7347</v>
-      </c>
-    </row>
-    <row r="7349" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7349" t="s">
-        <v>7348</v>
-      </c>
-    </row>
-    <row r="7350" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7350" t="s">
-        <v>7349</v>
-      </c>
-    </row>
-    <row r="7351" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7351" t="s">
-        <v>7350</v>
-      </c>
-    </row>
-    <row r="7352" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7352" t="s">
-        <v>7351</v>
-      </c>
-    </row>
-    <row r="7353" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7353" t="s">
-        <v>7352</v>
-      </c>
-    </row>
-    <row r="7354" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7354" t="s">
-        <v>7353</v>
-      </c>
-    </row>
-    <row r="7355" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7355" t="s">
-        <v>7354</v>
-      </c>
-    </row>
-    <row r="7356" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7356" t="s">
-        <v>7355</v>
-      </c>
-    </row>
-    <row r="7357" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7357" t="s">
-        <v>7356</v>
-      </c>
-    </row>
-    <row r="7358" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7358" t="s">
-        <v>7357</v>
-      </c>
-    </row>
-    <row r="7359" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7359" t="s">
-        <v>7358</v>
-      </c>
-    </row>
-    <row r="7360" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7360" t="s">
-        <v>7359</v>
-      </c>
-    </row>
-    <row r="7361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7361" t="s">
-        <v>7360</v>
-      </c>
-    </row>
-    <row r="7362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7362" t="s">
-        <v>7361</v>
-      </c>
-    </row>
-    <row r="7363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7363" t="s">
-        <v>7362</v>
-      </c>
-    </row>
-    <row r="7364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7364" t="s">
-        <v>7363</v>
-      </c>
-    </row>
-    <row r="7365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7365" t="s">
-        <v>7364</v>
-      </c>
-    </row>
-    <row r="7366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7366" t="s">
-        <v>7365</v>
-      </c>
-    </row>
-    <row r="7367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7367" t="s">
-        <v>7366</v>
-      </c>
-    </row>
-    <row r="7368" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7368" t="s">
-        <v>7367</v>
-      </c>
-    </row>
-    <row r="7369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7369" t="s">
-        <v>7368</v>
-      </c>
-    </row>
-    <row r="7370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7370" t="s">
-        <v>7369</v>
-      </c>
-    </row>
-    <row r="7371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7371" t="s">
-        <v>7370</v>
-      </c>
-    </row>
-    <row r="7372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7372" t="s">
-        <v>7371</v>
-      </c>
-    </row>
-    <row r="7373" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7373" t="s">
-        <v>7372</v>
-      </c>
-    </row>
-    <row r="7374" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7374" t="s">
-        <v>7373</v>
-      </c>
-    </row>
-    <row r="7375" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7375" t="s">
-        <v>7374</v>
-      </c>
-    </row>
-    <row r="7376" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7376" t="s">
-        <v>7375</v>
-      </c>
-    </row>
-    <row r="7377" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7377" t="s">
-        <v>7376</v>
-      </c>
-    </row>
-    <row r="7378" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7378" t="s">
-        <v>7377</v>
-      </c>
-    </row>
-    <row r="7379" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7379" t="s">
-        <v>7378</v>
-      </c>
-    </row>
-    <row r="7380" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7380" t="s">
-        <v>7379</v>
-      </c>
-    </row>
-    <row r="7381" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7381" t="s">
-        <v>7380</v>
-      </c>
-    </row>
-    <row r="7382" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7382" t="s">
-        <v>7381</v>
-      </c>
-    </row>
-    <row r="7383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7383" t="s">
-        <v>7382</v>
-      </c>
-    </row>
-    <row r="7384" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7384" t="s">
-        <v>7383</v>
-      </c>
-    </row>
-    <row r="7385" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7385" t="s">
-        <v>7384</v>
-      </c>
-    </row>
-    <row r="7386" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7386" t="s">
-        <v>7385</v>
-      </c>
-    </row>
-    <row r="7387" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7387" t="s">
-        <v>7386</v>
-      </c>
-    </row>
-    <row r="7388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7388" t="s">
-        <v>7387</v>
-      </c>
-    </row>
-    <row r="7389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7389" t="s">
-        <v>7388</v>
-      </c>
-    </row>
-    <row r="7390" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7390" t="s">
-        <v>7389</v>
-      </c>
-    </row>
-    <row r="7391" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7391" t="s">
-        <v>7390</v>
-      </c>
-    </row>
-    <row r="7392" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7392" t="s">
-        <v>7391</v>
-      </c>
-    </row>
-    <row r="7393" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7393" t="s">
-        <v>7392</v>
-      </c>
-    </row>
-    <row r="7394" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7394" t="s">
-        <v>7393</v>
-      </c>
-    </row>
-    <row r="7395" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7395" t="s">
-        <v>7394</v>
-      </c>
-    </row>
-    <row r="7396" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7396" t="s">
-        <v>7395</v>
-      </c>
-    </row>
-    <row r="7397" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7397" t="s">
-        <v>7396</v>
-      </c>
-    </row>
-    <row r="7398" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7398" t="s">
-        <v>7397</v>
-      </c>
-    </row>
-    <row r="7399" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7399" t="s">
-        <v>7398</v>
-      </c>
-    </row>
-    <row r="7400" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7400" t="s">
-        <v>7399</v>
-      </c>
-    </row>
-    <row r="7401" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7401" t="s">
-        <v>7400</v>
-      </c>
-    </row>
-    <row r="7402" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7402" t="s">
-        <v>7401</v>
-      </c>
-    </row>
-    <row r="7403" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7403" t="s">
-        <v>7402</v>
-      </c>
-    </row>
-    <row r="7404" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7404" t="s">
-        <v>7403</v>
-      </c>
-    </row>
-    <row r="7405" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7405" t="s">
-        <v>7404</v>
-      </c>
-    </row>
-    <row r="7406" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7406" t="s">
-        <v>7405</v>
-      </c>
-    </row>
-    <row r="7407" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7407" t="s">
-        <v>7406</v>
-      </c>
-    </row>
-    <row r="7408" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7408" t="s">
-        <v>7407</v>
-      </c>
-    </row>
-    <row r="7409" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7409" t="s">
-        <v>7408</v>
-      </c>
-    </row>
-    <row r="7410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7410" t="s">
-        <v>7409</v>
-      </c>
-    </row>
-    <row r="7411" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7411" t="s">
-        <v>7410</v>
-      </c>
-    </row>
-    <row r="7412" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7412" t="s">
-        <v>7411</v>
-      </c>
-    </row>
-    <row r="7413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7413" t="s">
-        <v>7412</v>
-      </c>
-    </row>
-    <row r="7414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7414" t="s">
-        <v>7413</v>
-      </c>
-    </row>
-    <row r="7415" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7415" t="s">
-        <v>7414</v>
-      </c>
-    </row>
-    <row r="7416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7416" t="s">
-        <v>7415</v>
-      </c>
-    </row>
-    <row r="7417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7417" t="s">
-        <v>7416</v>
-      </c>
-    </row>
-    <row r="7418" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7418" t="s">
-        <v>7417</v>
-      </c>
-    </row>
-    <row r="7419" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7419" t="s">
-        <v>7418</v>
-      </c>
-    </row>
-    <row r="7420" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7420" t="s">
-        <v>7419</v>
-      </c>
-    </row>
-    <row r="7421" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7421" t="s">
-        <v>7420</v>
-      </c>
-    </row>
-    <row r="7422" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7422" t="s">
-        <v>7421</v>
-      </c>
-    </row>
-    <row r="7423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7423" t="s">
-        <v>7422</v>
-      </c>
-    </row>
-    <row r="7424" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7424" t="s">
-        <v>7423</v>
-      </c>
-    </row>
-    <row r="7425" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7425" t="s">
-        <v>7424</v>
-      </c>
-    </row>
-    <row r="7426" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7426" t="s">
-        <v>7425</v>
-      </c>
-    </row>
-    <row r="7427" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7427" t="s">
-        <v>7426</v>
-      </c>
-    </row>
-    <row r="7428" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7428" t="s">
-        <v>7427</v>
-      </c>
-    </row>
-    <row r="7429" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7429" t="s">
-        <v>7428</v>
-      </c>
-    </row>
-    <row r="7430" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7430" t="s">
-        <v>7429</v>
-      </c>
-    </row>
-    <row r="7431" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7431" t="s">
-        <v>7430</v>
-      </c>
-    </row>
-    <row r="7432" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7432" t="s">
-        <v>7431</v>
-      </c>
-    </row>
-    <row r="7433" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7433" t="s">
-        <v>7432</v>
-      </c>
-    </row>
-    <row r="7434" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7434" t="s">
-        <v>7433</v>
-      </c>
-    </row>
-    <row r="7435" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7435" t="s">
-        <v>7434</v>
-      </c>
-    </row>
-    <row r="7436" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7436" t="s">
-        <v>7435</v>
-      </c>
-    </row>
-    <row r="7437" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7437" t="s">
-        <v>7436</v>
-      </c>
-    </row>
-    <row r="7438" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7438" t="s">
-        <v>7437</v>
-      </c>
-    </row>
-    <row r="7439" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7439" t="s">
-        <v>7438</v>
-      </c>
-    </row>
-    <row r="7440" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7440" t="s">
-        <v>7439</v>
-      </c>
-    </row>
-    <row r="7441" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7441" t="s">
-        <v>7440</v>
-      </c>
-    </row>
-    <row r="7442" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7442" t="s">
-        <v>7441</v>
-      </c>
-    </row>
-    <row r="7443" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7443" t="s">
-        <v>7442</v>
-      </c>
-    </row>
-    <row r="7444" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7444" t="s">
-        <v>7443</v>
-      </c>
-    </row>
-    <row r="7445" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7445" t="s">
-        <v>7444</v>
-      </c>
-    </row>
-    <row r="7446" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7446" t="s">
-        <v>7445</v>
-      </c>
-    </row>
-    <row r="7447" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7447" t="s">
-        <v>7446</v>
-      </c>
-    </row>
-    <row r="7448" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7448" t="s">
-        <v>7447</v>
-      </c>
-    </row>
-    <row r="7449" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7449" t="s">
-        <v>7448</v>
-      </c>
-    </row>
-    <row r="7450" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7450" t="s">
-        <v>7449</v>
-      </c>
-    </row>
-    <row r="7451" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7451" t="s">
-        <v>7450</v>
-      </c>
-    </row>
-    <row r="7452" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7452" t="s">
-        <v>7451</v>
-      </c>
-    </row>
-    <row r="7453" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7453" t="s">
-        <v>7452</v>
-      </c>
-    </row>
-    <row r="7454" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7454" t="s">
-        <v>7453</v>
-      </c>
-    </row>
-    <row r="7455" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7455" t="s">
-        <v>7454</v>
-      </c>
-    </row>
-    <row r="7456" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7456" t="s">
-        <v>7455</v>
-      </c>
-    </row>
-    <row r="7457" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7457" t="s">
-        <v>7456</v>
-      </c>
-    </row>
-    <row r="7458" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7458" t="s">
-        <v>7457</v>
-      </c>
-    </row>
-    <row r="7459" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7459" t="s">
-        <v>7458</v>
-      </c>
-    </row>
-    <row r="7460" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7460" t="s">
-        <v>7459</v>
-      </c>
-    </row>
-    <row r="7461" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7461" t="s">
-        <v>7460</v>
-      </c>
-    </row>
-    <row r="7462" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7462" t="s">
-        <v>7461</v>
-      </c>
-    </row>
-    <row r="7463" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7463" t="s">
-        <v>7462</v>
-      </c>
-    </row>
-    <row r="7464" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7464" t="s">
-        <v>7463</v>
-      </c>
-    </row>
-    <row r="7465" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7465" t="s">
-        <v>7464</v>
-      </c>
-    </row>
-    <row r="7466" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7466" t="s">
-        <v>7465</v>
-      </c>
-    </row>
-    <row r="7467" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7467" t="s">
-        <v>7466</v>
-      </c>
-    </row>
-    <row r="7468" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7468" t="s">
-        <v>7467</v>
-      </c>
-    </row>
-    <row r="7469" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7469" t="s">
-        <v>7468</v>
-      </c>
-    </row>
-    <row r="7470" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7470" t="s">
-        <v>7469</v>
-      </c>
-    </row>
-    <row r="7471" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7471" t="s">
-        <v>7470</v>
-      </c>
-    </row>
-    <row r="7472" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7472" t="s">
-        <v>7471</v>
-      </c>
-    </row>
-    <row r="7473" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7473" t="s">
-        <v>7472</v>
-      </c>
-    </row>
-    <row r="7474" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7474" t="s">
-        <v>7473</v>
-      </c>
-    </row>
-    <row r="7475" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7475" t="s">
-        <v>7474</v>
-      </c>
-    </row>
-    <row r="7476" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7476" t="s">
-        <v>7475</v>
-      </c>
-    </row>
-    <row r="7477" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7477" t="s">
-        <v>7476</v>
-      </c>
-    </row>
-    <row r="7478" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7478" t="s">
-        <v>7477</v>
-      </c>
-    </row>
-    <row r="7479" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7479" t="s">
-        <v>7478</v>
-      </c>
-    </row>
-    <row r="7480" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7480" t="s">
-        <v>7479</v>
-      </c>
-    </row>
-    <row r="7481" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7481" t="s">
-        <v>7480</v>
-      </c>
-    </row>
-    <row r="7482" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7482" t="s">
-        <v>7481</v>
-      </c>
-    </row>
-    <row r="7483" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7483" t="s">
-        <v>7482</v>
-      </c>
-    </row>
-    <row r="7484" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7484" t="s">
-        <v>7483</v>
-      </c>
-    </row>
-    <row r="7485" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7485" t="s">
-        <v>7484</v>
-      </c>
-    </row>
-    <row r="7486" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7486" t="s">
-        <v>7485</v>
-      </c>
-    </row>
-    <row r="7487" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7487" t="s">
-        <v>7486</v>
-      </c>
-    </row>
-    <row r="7488" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7488" t="s">
-        <v>7487</v>
-      </c>
-    </row>
-    <row r="7489" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7489" t="s">
-        <v>7488</v>
-      </c>
-    </row>
-    <row r="7490" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7490" t="s">
-        <v>7489</v>
-      </c>
-    </row>
-    <row r="7491" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7491" t="s">
-        <v>7490</v>
-      </c>
-    </row>
-    <row r="7492" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7492" t="s">
-        <v>7491</v>
-      </c>
-    </row>
-    <row r="7493" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7493" t="s">
-        <v>7492</v>
-      </c>
-    </row>
-    <row r="7494" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7494" t="s">
-        <v>7493</v>
-      </c>
-    </row>
-    <row r="7495" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7495" t="s">
-        <v>7494</v>
-      </c>
-    </row>
-    <row r="7496" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7496" t="s">
-        <v>7495</v>
-      </c>
-    </row>
-    <row r="7497" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7497" t="s">
-        <v>7496</v>
-      </c>
-    </row>
-    <row r="7498" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7498" t="s">
-        <v>7497</v>
-      </c>
-    </row>
-    <row r="7499" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7499" t="s">
-        <v>7498</v>
-      </c>
-    </row>
-    <row r="7500" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7500" t="s">
-        <v>7499</v>
-      </c>
-    </row>
-    <row r="7501" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7501" t="s">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="7502" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7502" t="s">
-        <v>7501</v>
-      </c>
-    </row>
-    <row r="7503" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7503" t="s">
-        <v>7502</v>
-      </c>
-    </row>
-    <row r="7504" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7504" t="s">
-        <v>7503</v>
-      </c>
-    </row>
-    <row r="7505" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7505" t="s">
-        <v>7504</v>
-      </c>
-    </row>
-    <row r="7506" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7506" t="s">
-        <v>7505</v>
-      </c>
-    </row>
-    <row r="7507" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7507" t="s">
-        <v>7506</v>
-      </c>
-    </row>
-    <row r="7508" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7508" t="s">
-        <v>7507</v>
-      </c>
-    </row>
-    <row r="7509" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7509" t="s">
-        <v>7508</v>
-      </c>
-    </row>
-    <row r="7510" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7510" t="s">
-        <v>7509</v>
-      </c>
-    </row>
-    <row r="7511" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7511" t="s">
-        <v>7510</v>
-      </c>
-    </row>
-    <row r="7512" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7512" t="s">
-        <v>7511</v>
-      </c>
-    </row>
-    <row r="7513" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7513" t="s">
-        <v>7512</v>
-      </c>
-    </row>
-    <row r="7514" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7514" t="s">
-        <v>7513</v>
-      </c>
-    </row>
-    <row r="7515" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7515" t="s">
-        <v>7514</v>
-      </c>
-    </row>
-    <row r="7516" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7516" t="s">
-        <v>7515</v>
-      </c>
-    </row>
-    <row r="7517" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7517" t="s">
-        <v>7516</v>
-      </c>
-    </row>
-    <row r="7518" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7518" t="s">
-        <v>7517</v>
-      </c>
-    </row>
-    <row r="7519" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7519" t="s">
-        <v>7518</v>
-      </c>
-    </row>
-    <row r="7520" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7520" t="s">
-        <v>7519</v>
-      </c>
-    </row>
-    <row r="7521" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7521" t="s">
-        <v>7520</v>
-      </c>
-    </row>
-    <row r="7522" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7522" t="s">
-        <v>7521</v>
-      </c>
-    </row>
-    <row r="7523" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7523" t="s">
-        <v>7522</v>
-      </c>
-    </row>
-    <row r="7524" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7524" t="s">
-        <v>7523</v>
-      </c>
-    </row>
-    <row r="7525" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7525" t="s">
-        <v>7524</v>
-      </c>
-    </row>
-    <row r="7526" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7526" t="s">
-        <v>7525</v>
-      </c>
-    </row>
-    <row r="7527" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7527" t="s">
-        <v>7526</v>
-      </c>
-    </row>
-    <row r="7528" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7528" t="s">
-        <v>7527</v>
-      </c>
-    </row>
-    <row r="7529" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7529" t="s">
-        <v>7528</v>
-      </c>
-    </row>
-    <row r="7530" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7530" t="s">
-        <v>7529</v>
-      </c>
-    </row>
-    <row r="7531" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7531" t="s">
-        <v>7530</v>
-      </c>
-    </row>
-    <row r="7532" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7532" t="s">
-        <v>7531</v>
-      </c>
-    </row>
-    <row r="7533" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7533" t="s">
-        <v>7532</v>
-      </c>
-    </row>
-    <row r="7534" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7534" t="s">
-        <v>7533</v>
-      </c>
-    </row>
-    <row r="7535" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7535" t="s">
-        <v>7534</v>
-      </c>
-    </row>
-    <row r="7536" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7536" t="s">
-        <v>7535</v>
-      </c>
-    </row>
-    <row r="7537" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7537" t="s">
-        <v>7536</v>
-      </c>
-    </row>
-    <row r="7538" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7538" t="s">
-        <v>7537</v>
-      </c>
-    </row>
-    <row r="7539" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7539" t="s">
-        <v>7538</v>
-      </c>
-    </row>
-    <row r="7540" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7540" t="s">
-        <v>7539</v>
-      </c>
-    </row>
-    <row r="7541" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7541" t="s">
-        <v>7540</v>
-      </c>
-    </row>
-    <row r="7542" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7542" t="s">
-        <v>7541</v>
-      </c>
-    </row>
-    <row r="7543" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7543" t="s">
-        <v>7542</v>
-      </c>
-    </row>
-    <row r="7544" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7544" t="s">
-        <v>7543</v>
-      </c>
-    </row>
-    <row r="7545" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7545" t="s">
-        <v>7544</v>
-      </c>
-    </row>
-    <row r="7546" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7546" t="s">
-        <v>7545</v>
-      </c>
-    </row>
-    <row r="7547" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7547" t="s">
-        <v>7546</v>
-      </c>
-    </row>
-    <row r="7548" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7548" t="s">
-        <v>7547</v>
-      </c>
-    </row>
-    <row r="7549" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7549" t="s">
-        <v>7548</v>
-      </c>
-    </row>
-    <row r="7550" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7550" t="s">
-        <v>7549</v>
-      </c>
-    </row>
-    <row r="7551" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7551" t="s">
-        <v>7550</v>
-      </c>
-    </row>
-    <row r="7552" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7552" t="s">
-        <v>7551</v>
-      </c>
-    </row>
-    <row r="7553" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7553" t="s">
-        <v>7552</v>
-      </c>
-    </row>
-    <row r="7554" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7554" t="s">
-        <v>7553</v>
-      </c>
-    </row>
-    <row r="7555" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7555" t="s">
-        <v>7554</v>
-      </c>
-    </row>
-    <row r="7556" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7556" t="s">
-        <v>7555</v>
-      </c>
-    </row>
-    <row r="7557" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7557" t="s">
-        <v>7556</v>
-      </c>
-    </row>
-    <row r="7558" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7558" t="s">
-        <v>7557</v>
-      </c>
-    </row>
-    <row r="7559" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7559" t="s">
-        <v>7558</v>
-      </c>
-    </row>
-    <row r="7560" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7560" t="s">
-        <v>7559</v>
-      </c>
-    </row>
-    <row r="7561" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7561" t="s">
-        <v>7560</v>
-      </c>
-    </row>
-    <row r="7562" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7562" t="s">
-        <v>7561</v>
-      </c>
-    </row>
-    <row r="7563" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7563" t="s">
-        <v>7562</v>
-      </c>
-    </row>
-    <row r="7564" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7564" t="s">
-        <v>7563</v>
-      </c>
-    </row>
-    <row r="7565" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7565" t="s">
-        <v>7564</v>
-      </c>
-    </row>
-    <row r="7566" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7566" t="s">
-        <v>7565</v>
-      </c>
-    </row>
-    <row r="7567" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7567" t="s">
-        <v>7566</v>
-      </c>
-    </row>
-    <row r="7568" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7568" t="s">
-        <v>7567</v>
-      </c>
-    </row>
-    <row r="7569" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7569" t="s">
-        <v>7568</v>
-      </c>
-    </row>
-    <row r="7570" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7570" t="s">
-        <v>7569</v>
-      </c>
-    </row>
-    <row r="7571" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7571" t="s">
-        <v>7570</v>
-      </c>
-    </row>
-    <row r="7572" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7572" t="s">
-        <v>7571</v>
-      </c>
-    </row>
-    <row r="7573" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7573" t="s">
-        <v>7572</v>
-      </c>
-    </row>
-    <row r="7574" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7574" t="s">
-        <v>7573</v>
-      </c>
-    </row>
-    <row r="7575" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7575" t="s">
-        <v>7574</v>
-      </c>
-    </row>
-    <row r="7576" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7576" t="s">
-        <v>7575</v>
-      </c>
-    </row>
-    <row r="7577" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7577" t="s">
-        <v>7576</v>
-      </c>
-    </row>
-    <row r="7578" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7578" t="s">
-        <v>7577</v>
-      </c>
-    </row>
-    <row r="7579" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7579" t="s">
-        <v>7578</v>
-      </c>
-    </row>
-    <row r="7580" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7580" t="s">
-        <v>7579</v>
-      </c>
-    </row>
-    <row r="7581" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7581" t="s">
-        <v>7580</v>
-      </c>
-    </row>
-    <row r="7582" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7582" t="s">
-        <v>7581</v>
-      </c>
-    </row>
-    <row r="7583" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7583" t="s">
-        <v>7582</v>
-      </c>
-    </row>
-    <row r="7584" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7584" t="s">
-        <v>7583</v>
-      </c>
-    </row>
-    <row r="7585" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7585" t="s">
-        <v>7584</v>
-      </c>
-    </row>
-    <row r="7586" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7586" t="s">
-        <v>7585</v>
-      </c>
-    </row>
-    <row r="7587" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7587" t="s">
-        <v>7586</v>
-      </c>
-    </row>
-    <row r="7588" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7588" t="s">
-        <v>7587</v>
-      </c>
-    </row>
-    <row r="7589" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7589" t="s">
-        <v>7588</v>
-      </c>
-    </row>
-    <row r="7590" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7590" t="s">
-        <v>7589</v>
-      </c>
-    </row>
-    <row r="7591" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7591" t="s">
-        <v>7590</v>
-      </c>
-    </row>
-    <row r="7592" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7592" t="s">
-        <v>7591</v>
-      </c>
-    </row>
-    <row r="7593" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7593" t="s">
-        <v>7592</v>
-      </c>
-    </row>
-    <row r="7594" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7594" t="s">
-        <v>7593</v>
-      </c>
-    </row>
-    <row r="7595" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7595" t="s">
-        <v>7594</v>
-      </c>
-    </row>
-    <row r="7596" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7596" t="s">
-        <v>7595</v>
-      </c>
-    </row>
-    <row r="7597" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7597" t="s">
-        <v>7596</v>
-      </c>
-    </row>
-    <row r="7598" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7598" t="s">
-        <v>7597</v>
-      </c>
-    </row>
-    <row r="7599" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7599" t="s">
-        <v>7598</v>
-      </c>
-    </row>
-    <row r="7600" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7600" t="s">
-        <v>7599</v>
-      </c>
-    </row>
-    <row r="7601" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7601" t="s">
-        <v>7600</v>
-      </c>
-    </row>
-    <row r="7602" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7602" t="s">
-        <v>7601</v>
-      </c>
-    </row>
-    <row r="7603" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7603" t="s">
-        <v>7602</v>
-      </c>
-    </row>
-    <row r="7604" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7604" t="s">
-        <v>7603</v>
-      </c>
-    </row>
-    <row r="7605" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7605" t="s">
-        <v>7604</v>
-      </c>
-    </row>
-    <row r="7606" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7606" t="s">
-        <v>7605</v>
-      </c>
-    </row>
-    <row r="7607" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7607" t="s">
-        <v>7606</v>
-      </c>
-    </row>
-    <row r="7608" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7608" t="s">
-        <v>7607</v>
-      </c>
-    </row>
-    <row r="7609" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7609" t="s">
-        <v>7608</v>
-      </c>
-    </row>
-    <row r="7610" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7610" t="s">
-        <v>7609</v>
-      </c>
-    </row>
-    <row r="7611" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7611" t="s">
-        <v>7610</v>
-      </c>
-    </row>
-    <row r="7612" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7612" t="s">
-        <v>7611</v>
-      </c>
-    </row>
-    <row r="7613" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7613" t="s">
-        <v>7612</v>
-      </c>
-    </row>
-    <row r="7614" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7614" t="s">
-        <v>7613</v>
-      </c>
-    </row>
-    <row r="7615" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7615" t="s">
-        <v>7614</v>
-      </c>
-    </row>
-    <row r="7616" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7616" t="s">
-        <v>7615</v>
-      </c>
-    </row>
-    <row r="7617" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7617" t="s">
-        <v>7616</v>
-      </c>
-    </row>
-    <row r="7618" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7618" t="s">
-        <v>7617</v>
-      </c>
-    </row>
-    <row r="7619" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7619" t="s">
-        <v>7618</v>
-      </c>
-    </row>
-    <row r="7620" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7620" t="s">
-        <v>7619</v>
-      </c>
-    </row>
-    <row r="7621" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7621" t="s">
-        <v>7620</v>
-      </c>
-    </row>
-    <row r="7622" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7622" t="s">
-        <v>7621</v>
-      </c>
-    </row>
-    <row r="7623" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7623" t="s">
-        <v>7622</v>
-      </c>
-    </row>
-    <row r="7624" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7624" t="s">
-        <v>7623</v>
-      </c>
-    </row>
-    <row r="7625" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7625" t="s">
-        <v>7624</v>
-      </c>
-    </row>
-    <row r="7626" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7626" t="s">
-        <v>7625</v>
-      </c>
-    </row>
-    <row r="7627" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7627" t="s">
-        <v>7626</v>
-      </c>
-    </row>
-    <row r="7628" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7628" t="s">
-        <v>7627</v>
-      </c>
-    </row>
-    <row r="7629" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7629" t="s">
-        <v>7628</v>
-      </c>
-    </row>
-    <row r="7630" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7630" t="s">
-        <v>7629</v>
-      </c>
-    </row>
-    <row r="7631" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7631" t="s">
-        <v>7630</v>
-      </c>
-    </row>
-    <row r="7632" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7632" t="s">
-        <v>7631</v>
-      </c>
-    </row>
-    <row r="7633" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7633" t="s">
-        <v>7632</v>
-      </c>
-    </row>
-    <row r="7634" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7634" t="s">
-        <v>7633</v>
-      </c>
-    </row>
-    <row r="7635" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7635" t="s">
-        <v>7634</v>
-      </c>
-    </row>
-    <row r="7636" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7636" t="s">
-        <v>7635</v>
-      </c>
-    </row>
-    <row r="7637" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7637" t="s">
-        <v>7636</v>
-      </c>
-    </row>
-    <row r="7638" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7638" t="s">
-        <v>7637</v>
-      </c>
-    </row>
-    <row r="7639" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7639" t="s">
-        <v>7638</v>
-      </c>
-    </row>
-    <row r="7640" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7640" t="s">
-        <v>7639</v>
-      </c>
-    </row>
-    <row r="7641" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7641" t="s">
-        <v>7640</v>
-      </c>
-    </row>
-    <row r="7642" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7642" t="s">
-        <v>7641</v>
-      </c>
-    </row>
-    <row r="7643" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7643" t="s">
-        <v>7642</v>
-      </c>
-    </row>
-    <row r="7644" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7644" t="s">
-        <v>7643</v>
-      </c>
-    </row>
-    <row r="7645" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7645" t="s">
-        <v>7644</v>
-      </c>
-    </row>
-    <row r="7646" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7646" t="s">
-        <v>7645</v>
-      </c>
-    </row>
-    <row r="7647" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7647" t="s">
-        <v>7646</v>
-      </c>
-    </row>
-    <row r="7648" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7648" t="s">
-        <v>7647</v>
-      </c>
-    </row>
-    <row r="7649" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7649" t="s">
-        <v>7648</v>
-      </c>
-    </row>
-    <row r="7650" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7650" t="s">
-        <v>7649</v>
-      </c>
-    </row>
-    <row r="7651" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7651" t="s">
-        <v>7650</v>
-      </c>
-    </row>
-    <row r="7652" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7652" t="s">
-        <v>7651</v>
-      </c>
-    </row>
-    <row r="7653" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7653" t="s">
-        <v>7652</v>
-      </c>
-    </row>
-    <row r="7654" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7654" t="s">
-        <v>7653</v>
-      </c>
-    </row>
-    <row r="7655" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7655" t="s">
-        <v>7654</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>